<commit_message>
complted till report submitting
</commit_message>
<xml_diff>
--- a/resultExcel.xlsx
+++ b/resultExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>Index</t>
   </si>
@@ -165,6 +165,75 @@
   </si>
   <si>
     <t>₹25,762</t>
+  </si>
+  <si>
+    <t>Lavish Rectangular Metal Coffee Table In Powder Coating Finish</t>
+  </si>
+  <si>
+    <t>₹23,220</t>
+  </si>
+  <si>
+    <t>Frazer Rectangular Metal Coffee Table In Powder Coating Finish</t>
+  </si>
+  <si>
+    <t>₹25,451</t>
+  </si>
+  <si>
+    <t>Marten Rectangular Metal Coffee Table In Powder Coating Finish</t>
+  </si>
+  <si>
+    <t>₹23,853</t>
+  </si>
+  <si>
+    <t>Alix Rectangular Metal Coffee Table In Stainless Steel Finish</t>
+  </si>
+  <si>
+    <t>₹19,763</t>
+  </si>
+  <si>
+    <t>Hazel Round Metal Coffee Table In Powder Coating Finish</t>
+  </si>
+  <si>
+    <t>Peter Square Metal Coffee Table In Powder Coating Finish</t>
+  </si>
+  <si>
+    <t>Doug Square Metal Coffee Table In Powder Coating Finish</t>
+  </si>
+  <si>
+    <t>Angel Round Metal Coffee Table In Powder Coating Finish</t>
+  </si>
+  <si>
+    <t>₹20,656</t>
+  </si>
+  <si>
+    <t>₹19,999</t>
+  </si>
+  <si>
+    <t>Blane Square Solid Wood Coffee Table In Antique Grey Finish</t>
+  </si>
+  <si>
+    <t>Nashville Round Solid Wood Coffee Table In Antique Grey Finish</t>
+  </si>
+  <si>
+    <t>₹18,998</t>
+  </si>
+  <si>
+    <t>Blane Square Solid Wood Coffee Table In Walnut Finish</t>
+  </si>
+  <si>
+    <t>Nashville Round Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>Irish Rectangular Solid Wood Coffee Table In Walnut Finish</t>
+  </si>
+  <si>
+    <t>Irish Rectangular Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>Milan Square Solid Wood Coffee Table In Walnut Finish</t>
+  </si>
+  <si>
+    <t>Montreal Square Solid Wood Coffee Table In Walnut Finish</t>
   </si>
 </sst>
 </file>
@@ -209,7 +278,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -556,6 +625,336 @@
         <v>50</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="n" s="0">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="0">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n" s="0">
+        <v>35.0</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="0">
+        <v>39.0</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="0">
+        <v>42.0</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="0">
+        <v>43.0</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n" s="0">
+        <v>44.0</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n" s="0">
+        <v>47.0</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n" s="0">
+        <v>48.0</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n" s="0">
+        <v>49.0</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n" s="0">
+        <v>51.0</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n" s="0">
+        <v>52.0</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n" s="0">
+        <v>53.0</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n" s="0">
+        <v>54.0</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n" s="0">
+        <v>55.0</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n" s="0">
+        <v>56.0</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n" s="0">
+        <v>57.0</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n" s="0">
+        <v>58.0</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n" s="0">
+        <v>59.0</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
created of result is successfull
</commit_message>
<xml_diff>
--- a/resultExcel.xlsx
+++ b/resultExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Index</t>
   </si>
@@ -165,75 +165,6 @@
   </si>
   <si>
     <t>₹25,762</t>
-  </si>
-  <si>
-    <t>₹23,220</t>
-  </si>
-  <si>
-    <t>Lavish Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>Frazer Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹25,451</t>
-  </si>
-  <si>
-    <t>Marten Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹23,853</t>
-  </si>
-  <si>
-    <t>Alix Rectangular Metal Coffee Table In Stainless Steel Finish</t>
-  </si>
-  <si>
-    <t>₹19,763</t>
-  </si>
-  <si>
-    <t>Hazel Round Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>Peter Square Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>Doug Square Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>Angel Round Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹20,656</t>
-  </si>
-  <si>
-    <t>₹19,999</t>
-  </si>
-  <si>
-    <t>Blane Square Solid Wood Coffee Table In Antique Grey Finish</t>
-  </si>
-  <si>
-    <t>Nashville Round Solid Wood Coffee Table In Antique Grey Finish</t>
-  </si>
-  <si>
-    <t>₹18,998</t>
-  </si>
-  <si>
-    <t>Blane Square Solid Wood Coffee Table In Walnut Finish</t>
-  </si>
-  <si>
-    <t>Nashville Round Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>Irish Rectangular Solid Wood Coffee Table In Walnut Finish</t>
-  </si>
-  <si>
-    <t>Irish Rectangular Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>Milan Square Solid Wood Coffee Table In Walnut Finish</t>
-  </si>
-  <si>
-    <t>Montreal Square Solid Wood Coffee Table In Walnut Finish</t>
   </si>
 </sst>
 </file>
@@ -278,7 +209,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -625,336 +556,6 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="n" s="0">
-        <v>31.0</v>
-      </c>
-      <c r="B32" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="C32" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n" s="0">
-        <v>32.0</v>
-      </c>
-      <c r="B33" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n" s="0">
-        <v>33.0</v>
-      </c>
-      <c r="B34" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C34" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n" s="0">
-        <v>34.0</v>
-      </c>
-      <c r="B35" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n" s="0">
-        <v>35.0</v>
-      </c>
-      <c r="B36" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="C36" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n" s="0">
-        <v>36.0</v>
-      </c>
-      <c r="B37" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="C37" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n" s="0">
-        <v>37.0</v>
-      </c>
-      <c r="B38" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="C38" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n" s="0">
-        <v>38.0</v>
-      </c>
-      <c r="B39" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="C39" t="s" s="0">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n" s="0">
-        <v>39.0</v>
-      </c>
-      <c r="B40" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="C40" t="s" s="0">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n" s="0">
-        <v>40.0</v>
-      </c>
-      <c r="B41" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C41" t="s" s="0">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n" s="0">
-        <v>41.0</v>
-      </c>
-      <c r="B42" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="C42" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n" s="0">
-        <v>42.0</v>
-      </c>
-      <c r="B43" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="C43" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n" s="0">
-        <v>43.0</v>
-      </c>
-      <c r="B44" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="C44" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n" s="0">
-        <v>44.0</v>
-      </c>
-      <c r="B45" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="C45" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n" s="0">
-        <v>45.0</v>
-      </c>
-      <c r="B46" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="C46" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n" s="0">
-        <v>46.0</v>
-      </c>
-      <c r="B47" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="C47" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n" s="0">
-        <v>47.0</v>
-      </c>
-      <c r="B48" t="s" s="0">
-        <v>66</v>
-      </c>
-      <c r="C48" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n" s="0">
-        <v>48.0</v>
-      </c>
-      <c r="B49" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C49" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n" s="0">
-        <v>49.0</v>
-      </c>
-      <c r="B50" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="C50" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n" s="0">
-        <v>50.0</v>
-      </c>
-      <c r="B51" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="C51" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n" s="0">
-        <v>51.0</v>
-      </c>
-      <c r="B52" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="C52" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n" s="0">
-        <v>52.0</v>
-      </c>
-      <c r="B53" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="C53" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n" s="0">
-        <v>53.0</v>
-      </c>
-      <c r="B54" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="C54" t="s" s="0">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n" s="0">
-        <v>54.0</v>
-      </c>
-      <c r="B55" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="C55" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n" s="0">
-        <v>55.0</v>
-      </c>
-      <c r="B56" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="C56" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n" s="0">
-        <v>56.0</v>
-      </c>
-      <c r="B57" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="C57" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n" s="0">
-        <v>57.0</v>
-      </c>
-      <c r="B58" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="C58" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n" s="0">
-        <v>58.0</v>
-      </c>
-      <c r="B59" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="C59" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n" s="0">
-        <v>59.0</v>
-      </c>
-      <c r="B60" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="C60" t="s" s="0">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n" s="0">
-        <v>60.0</v>
-      </c>
-      <c r="B61" t="s" s="0">
-        <v>73</v>
-      </c>
-      <c r="C61" t="s" s="0">
-        <v>42</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
testing for the headless run
</commit_message>
<xml_diff>
--- a/resultExcel.xlsx
+++ b/resultExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Index</t>
   </si>
@@ -23,6 +23,24 @@
     <t>Price</t>
   </si>
   <si>
+    <t>Meridian Round Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹5,939</t>
+  </si>
+  <si>
+    <t>Adele Rectangular Engineered Wood Coffee Table In Classic Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹2,927</t>
+  </si>
+  <si>
+    <t>Awdry Rectangular Engineered Wood Coffee Table In Sonoma Oak Finish</t>
+  </si>
+  <si>
+    <t>₹2,903</t>
+  </si>
+  <si>
     <t>Altura Rectangular Solid Wood Coffee Table In Two Tone Finish</t>
   </si>
   <si>
@@ -59,27 +77,60 @@
     <t>₹15,317</t>
   </si>
   <si>
+    <t>Dyson Abstract Metal Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹7,679</t>
+  </si>
+  <si>
     <t>Ivara Rectangular Solid Wood Coffee Table In Natural Finish</t>
   </si>
   <si>
     <t>₹16,049</t>
   </si>
   <si>
+    <t>Botwin Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
+  </si>
+  <si>
+    <t>₹9,647</t>
+  </si>
+  <si>
     <t>Zephyr Rectangular Solid Wood Coffee Table In Teak Finish</t>
   </si>
   <si>
     <t>₹14,104</t>
   </si>
   <si>
+    <t>Fring Engineered Wood Side Table In Matte Finish</t>
+  </si>
+  <si>
+    <t>₹2,399</t>
+  </si>
+  <si>
     <t>Claire Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
   </si>
   <si>
+    <t>Botwin Rectangular Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
     <t>Epsilon Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
   </si>
   <si>
     <t>₹11,384</t>
   </si>
   <si>
+    <t>Dyson Rectangular Metal Coffee Table In Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹10,529</t>
+  </si>
+  <si>
+    <t>Gustowe Rectangular Engineered Wood Coffee Table In Matte Finish</t>
+  </si>
+  <si>
+    <t>₹2,279</t>
+  </si>
+  <si>
     <t>Striado Rectangular Solid Wood Coffee Table In Mahogany Finish</t>
   </si>
   <si>
@@ -89,12 +140,33 @@
     <t>₹15,677</t>
   </si>
   <si>
+    <t>₹8,374</t>
+  </si>
+  <si>
     <t>Sylvie Rectangular Solid Wood Coffee Table In Natural Finish</t>
   </si>
   <si>
     <t>₹11,839</t>
   </si>
   <si>
+    <t>Florence Oval Solid Wood Coffee Table In Teak Finish</t>
+  </si>
+  <si>
+    <t>₹10,223</t>
+  </si>
+  <si>
+    <t>Liam Rectangular Engineered Wood Coffee Table In Dark Wenge Finish</t>
+  </si>
+  <si>
+    <t>₹3,817</t>
+  </si>
+  <si>
+    <t>Reeves Rectangular Engineered Wood Coffee Table In Rustic Walnut Finish</t>
+  </si>
+  <si>
+    <t>₹5,543</t>
+  </si>
+  <si>
     <t>Nitara Oval Solid Wood Coffee Table In Teak Finish</t>
   </si>
   <si>
@@ -104,67 +176,13 @@
     <t>Renesme Rectangular Solid Wood Coffee Table In Teak Finish</t>
   </si>
   <si>
+    <t>Odette Square Solid Wood Coffee Table In Honey Oak Finish</t>
+  </si>
+  <si>
+    <t>₹5,919</t>
+  </si>
+  <si>
     <t>Epsilon Rectangular Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>Anny Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹27,284</t>
-  </si>
-  <si>
-    <t>Robert Rectangular Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹13,999</t>
-  </si>
-  <si>
-    <t>Blane Square Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹19,499</t>
-  </si>
-  <si>
-    <t>Rigby Round Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹17,273</t>
-  </si>
-  <si>
-    <t>Milan Square Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹13,498</t>
-  </si>
-  <si>
-    <t>Montreal Square Solid Wood Coffee Table In Teak Finish</t>
-  </si>
-  <si>
-    <t>₹11,498</t>
-  </si>
-  <si>
-    <t>Leena Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹28,648</t>
-  </si>
-  <si>
-    <t>Faye Rectangular Metal Coffee Table In Stainless Steel Finish</t>
-  </si>
-  <si>
-    <t>Harry Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>Laatto Rectangular Solid Wood Coffee Table In Melamine Finish</t>
-  </si>
-  <si>
-    <t>₹22,040</t>
-  </si>
-  <si>
-    <t>Daniel Rectangular Metal Coffee Table In Powder Coating Finish</t>
-  </si>
-  <si>
-    <t>₹25,762</t>
   </si>
 </sst>
 </file>
@@ -322,7 +340,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -330,10 +348,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -341,10 +359,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -352,10 +370,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
@@ -363,10 +381,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -374,10 +392,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
@@ -385,10 +403,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -396,10 +414,10 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18">
@@ -407,10 +425,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -418,10 +436,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
@@ -429,10 +447,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
@@ -440,10 +458,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22">
@@ -451,10 +469,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23">
@@ -462,10 +480,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24">
@@ -473,10 +491,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25">
@@ -484,10 +502,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
@@ -495,10 +513,10 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27">
@@ -506,10 +524,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28">
@@ -517,10 +535,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29">
@@ -528,10 +546,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>44</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30">
@@ -539,10 +557,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31">
@@ -550,10 +568,10 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>